<commit_message>
add distance to closest airport
</commit_message>
<xml_diff>
--- a/data/Addresses.xlsx
+++ b/data/Addresses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS4529\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS4529\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBC0470-971F-4CF2-9903-5A029DB85506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B37A797-3858-42D0-A85B-181DBAF32A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Domicile</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Northern Ireland</t>
+  </si>
+  <si>
+    <t>CF11 8AZ</t>
+  </si>
+  <si>
+    <t>Wales</t>
   </si>
 </sst>
 </file>
@@ -378,9 +384,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -421,6 +429,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>